<commit_message>
ajuste de 1 minuto a cada 3 requisicao
</commit_message>
<xml_diff>
--- a/Planilha_CNPJ.xlsx
+++ b/Planilha_CNPJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor Emanuell\OneDrive\Área de Trabalho\API Receita Federal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEDB2EE-E88E-4162-8498-E8D302383D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2090A4F4-5946-4F1D-8320-50A69ACF797C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC2DCA5F-DC70-4DD2-94F8-232A76390F9A}"/>
   </bookViews>
@@ -80,10 +80,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9E3733-595A-4691-97BD-294353F73527}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,8 +416,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>53405671000107</v>
+      <c r="A2" s="3">
+        <v>29148959000150</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -432,6 +433,11 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>53405671000107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>51041667000173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>